<commit_message>
Bucketing functionality hacked in
</commit_message>
<xml_diff>
--- a/Insiderate/output.xlsx
+++ b/Insiderate/output.xlsx
@@ -10,6 +10,7 @@
     <s:sheet name="WBTAveDay" sheetId="1" r:id="rId1"/>
     <s:sheet name="EnergyAveDay" sheetId="2" r:id="rId2"/>
     <s:sheet name="BandData" sheetId="3" r:id="rId3"/>
+    <s:sheet name="Bucketed Usage" sheetId="4" r:id="rId4"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -43,7 +44,13 @@
     <t>Elec-Mean</t>
   </si>
   <si>
+    <t>Elec-Occ</t>
+  </si>
+  <si>
     <t>Elec-StDev</t>
+  </si>
+  <si>
+    <t>Elec-Unocc</t>
   </si>
   <si>
     <t>Elec-Upper</t>
@@ -82,7 +89,13 @@
     <t>Stea-Mean</t>
   </si>
   <si>
+    <t>Stea-Occ</t>
+  </si>
+  <si>
     <t>Stea-StDev</t>
+  </si>
+  <si>
+    <t>Stea-Unocc</t>
   </si>
   <si>
     <t>Stea-Upper</t>
@@ -500,22 +513,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c s="2" r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c s="2" r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c s="2" r="D1" t="s">
         <v>31</v>
       </c>
-      <c s="2" r="C1" t="s">
+      <c s="2" r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c s="2" r="F1" t="s">
         <v>32</v>
       </c>
-      <c s="2" r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c s="2" r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c s="2" r="F1" t="s">
-        <v>28</v>
-      </c>
       <c s="2" r="G1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1104,10 +1117,10 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c s="2" r="B1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c s="2" r="C1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c s="2" r="D1" t="s">
         <v>2</v>
@@ -1122,22 +1135,22 @@
         <v>5</v>
       </c>
       <c s="2" r="H1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c s="2" r="I1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c s="2" r="J1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c s="2" r="K1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c s="2" r="L1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c s="2" r="M1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -5118,40 +5131,40 @@
         <v>7</v>
       </c>
       <c s="2" r="D1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c s="2" r="E1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c s="2" r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c s="2" r="G1" t="s">
         <v>11</v>
-      </c>
-      <c s="2" r="G1" t="s">
-        <v>9</v>
       </c>
       <c s="2" r="H1" t="s">
         <v>6</v>
       </c>
       <c s="2" r="I1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c s="2" r="J1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c s="2" r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c s="2" r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c s="2" r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c s="2" r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c s="2" r="O1" t="s">
         <v>21</v>
-      </c>
-      <c s="2" r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c s="2" r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c s="2" r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c s="2" r="O1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -22316,4 +22329,931 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:E54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c s="2" r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c s="2" r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c s="2" r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c s="2" r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c s="2" r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c s="1" r="A3" t="n">
+        <v>41280.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11252.879999999996</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7435.439999999998</v>
+      </c>
+      <c r="D3" t="n">
+        <v>11252.879999999996</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7435.439999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c s="1" r="A4" t="n">
+        <v>41287.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>16595.760000000013</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9991.919999999993</v>
+      </c>
+      <c r="D4" t="n">
+        <v>16595.760000000013</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9991.919999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c s="1" r="A5" t="n">
+        <v>41294.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>18249.359999999997</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11644.559999999987</v>
+      </c>
+      <c r="D5" t="n">
+        <v>18249.359999999997</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11644.559999999987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c s="1" r="A6" t="n">
+        <v>41301.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>17347.199999999997</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11670.479999999998</v>
+      </c>
+      <c r="D6" t="n">
+        <v>17347.199999999997</v>
+      </c>
+      <c r="E6" t="n">
+        <v>11670.479999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c s="1" r="A7" t="n">
+        <v>41308.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>18189.600000000002</v>
+      </c>
+      <c r="C7" t="n">
+        <v>11113.679999999998</v>
+      </c>
+      <c r="D7" t="n">
+        <v>18189.600000000002</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11113.679999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c s="1" r="A8" t="n">
+        <v>41315.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>17973.839999999986</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11142.720000000003</v>
+      </c>
+      <c r="D8" t="n">
+        <v>17973.839999999986</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11142.720000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c s="1" r="A9" t="n">
+        <v>41322.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>18184.319999999996</v>
+      </c>
+      <c r="C9" t="n">
+        <v>11189.759999999986</v>
+      </c>
+      <c r="D9" t="n">
+        <v>18184.319999999996</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11189.759999999986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c s="1" r="A10" t="n">
+        <v>41329.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>17351.28</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10848.239999999993</v>
+      </c>
+      <c r="D10" t="n">
+        <v>17351.28</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10848.239999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c s="1" r="A11" t="n">
+        <v>41336.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>17763.59999999999</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10870.319999999996</v>
+      </c>
+      <c r="D11" t="n">
+        <v>17763.59999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10870.319999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c s="1" r="A12" t="n">
+        <v>41343.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>17715.600000000006</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10544.639999999992</v>
+      </c>
+      <c r="D12" t="n">
+        <v>17715.600000000006</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10544.639999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c s="1" r="A13" t="n">
+        <v>41350.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>17233.439999999988</v>
+      </c>
+      <c r="C13" t="n">
+        <v>10443.12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>17233.439999999988</v>
+      </c>
+      <c r="E13" t="n">
+        <v>10443.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c s="1" r="A14" t="n">
+        <v>41357.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>17514.00000000001</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10575.36</v>
+      </c>
+      <c r="D14" t="n">
+        <v>17514.00000000001</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10575.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c s="1" r="A15" t="n">
+        <v>41364.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>17358.959999999995</v>
+      </c>
+      <c r="C15" t="n">
+        <v>11339.519999999986</v>
+      </c>
+      <c r="D15" t="n">
+        <v>17358.959999999995</v>
+      </c>
+      <c r="E15" t="n">
+        <v>11339.519999999986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c s="1" r="A16" t="n">
+        <v>41371.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>17531.76000000001</v>
+      </c>
+      <c r="C16" t="n">
+        <v>11273.280000000006</v>
+      </c>
+      <c r="D16" t="n">
+        <v>17531.76000000001</v>
+      </c>
+      <c r="E16" t="n">
+        <v>11273.280000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c s="1" r="A17" t="n">
+        <v>41378.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>17724.96</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10608.480000000001</v>
+      </c>
+      <c r="D17" t="n">
+        <v>17724.96</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10608.480000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c s="1" r="A18" t="n">
+        <v>41385.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17752.08</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10880.639999999998</v>
+      </c>
+      <c r="D18" t="n">
+        <v>17752.08</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10880.639999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c s="1" r="A19" t="n">
+        <v>41392.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17689.199999999997</v>
+      </c>
+      <c r="C19" t="n">
+        <v>10676.400000000014</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17689.199999999997</v>
+      </c>
+      <c r="E19" t="n">
+        <v>10676.400000000014</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c s="1" r="A20" t="n">
+        <v>41399.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>17281.68</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10107.360000000006</v>
+      </c>
+      <c r="D20" t="n">
+        <v>17281.68</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10107.360000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c s="1" r="A21" t="n">
+        <v>41406.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>17271.84</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10043.280000000002</v>
+      </c>
+      <c r="D21" t="n">
+        <v>17271.84</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10043.280000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c s="1" r="A22" t="n">
+        <v>41413.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>17381.760000000002</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10251.600000000004</v>
+      </c>
+      <c r="D22" t="n">
+        <v>17381.760000000002</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10251.600000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c s="1" r="A23" t="n">
+        <v>41420.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>17549.27999999999</v>
+      </c>
+      <c r="C23" t="n">
+        <v>10121.040000000008</v>
+      </c>
+      <c r="D23" t="n">
+        <v>17549.27999999999</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10121.040000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c s="1" r="A24" t="n">
+        <v>41427.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>15844.560000000007</v>
+      </c>
+      <c r="C24" t="n">
+        <v>9768.720000000005</v>
+      </c>
+      <c r="D24" t="n">
+        <v>15844.560000000007</v>
+      </c>
+      <c r="E24" t="n">
+        <v>9768.720000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c s="1" r="A25" t="n">
+        <v>41434.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>19764.960000000003</v>
+      </c>
+      <c r="C25" t="n">
+        <v>10454.88000000001</v>
+      </c>
+      <c r="D25" t="n">
+        <v>19764.960000000003</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10454.88000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c s="1" r="A26" t="n">
+        <v>41441.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>19113.120000000006</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10611.120000000004</v>
+      </c>
+      <c r="D26" t="n">
+        <v>19113.120000000006</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10611.120000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c s="1" r="A27" t="n">
+        <v>41448.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>19248.239999999994</v>
+      </c>
+      <c r="C27" t="n">
+        <v>10474.080000000009</v>
+      </c>
+      <c r="D27" t="n">
+        <v>19248.239999999994</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10474.080000000009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c s="1" r="A28" t="n">
+        <v>41455.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>18042.24000000002</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10617.600000000002</v>
+      </c>
+      <c r="D28" t="n">
+        <v>18042.24000000002</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10617.600000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c s="1" r="A29" t="n">
+        <v>41462.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>16016.400000000007</v>
+      </c>
+      <c r="C29" t="n">
+        <v>9829.199999999999</v>
+      </c>
+      <c r="D29" t="n">
+        <v>16016.400000000007</v>
+      </c>
+      <c r="E29" t="n">
+        <v>9829.199999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c s="1" r="A30" t="n">
+        <v>41469.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>18574.319999999985</v>
+      </c>
+      <c r="C30" t="n">
+        <v>11116.080000000002</v>
+      </c>
+      <c r="D30" t="n">
+        <v>18574.319999999985</v>
+      </c>
+      <c r="E30" t="n">
+        <v>11116.080000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c s="1" r="A31" t="n">
+        <v>41476.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>18980.63999999997</v>
+      </c>
+      <c r="C31" t="n">
+        <v>11166.000000000002</v>
+      </c>
+      <c r="D31" t="n">
+        <v>18980.63999999997</v>
+      </c>
+      <c r="E31" t="n">
+        <v>11166.000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c s="1" r="A32" t="n">
+        <v>41483.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>17852.64</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10284.480000000007</v>
+      </c>
+      <c r="D32" t="n">
+        <v>17852.64</v>
+      </c>
+      <c r="E32" t="n">
+        <v>10284.480000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c s="1" r="A33" t="n">
+        <v>41490.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>17306.400000000005</v>
+      </c>
+      <c r="C33" t="n">
+        <v>10058.640000000003</v>
+      </c>
+      <c r="D33" t="n">
+        <v>17306.400000000005</v>
+      </c>
+      <c r="E33" t="n">
+        <v>10058.640000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c s="1" r="A34" t="n">
+        <v>41497.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>17120.879999999986</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10259.759999999991</v>
+      </c>
+      <c r="D34" t="n">
+        <v>17120.879999999986</v>
+      </c>
+      <c r="E34" t="n">
+        <v>10259.759999999991</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c s="1" r="A35" t="n">
+        <v>41504.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>17003.520000000015</v>
+      </c>
+      <c r="C35" t="n">
+        <v>9873.359999999997</v>
+      </c>
+      <c r="D35" t="n">
+        <v>17003.520000000015</v>
+      </c>
+      <c r="E35" t="n">
+        <v>9873.359999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c s="1" r="A36" t="n">
+        <v>41511.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>16963.91999999999</v>
+      </c>
+      <c r="C36" t="n">
+        <v>9810.239999999996</v>
+      </c>
+      <c r="D36" t="n">
+        <v>16963.91999999999</v>
+      </c>
+      <c r="E36" t="n">
+        <v>9810.239999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c s="1" r="A37" t="n">
+        <v>41518.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>17068.320000000007</v>
+      </c>
+      <c r="C37" t="n">
+        <v>9924.480000000001</v>
+      </c>
+      <c r="D37" t="n">
+        <v>17068.320000000007</v>
+      </c>
+      <c r="E37" t="n">
+        <v>9924.480000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c s="1" r="A38" t="n">
+        <v>41525.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>16421.760000000006</v>
+      </c>
+      <c r="C38" t="n">
+        <v>9541.919999999993</v>
+      </c>
+      <c r="D38" t="n">
+        <v>16421.760000000006</v>
+      </c>
+      <c r="E38" t="n">
+        <v>9541.919999999993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c s="1" r="A39" t="n">
+        <v>41532.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>17500.079999999998</v>
+      </c>
+      <c r="C39" t="n">
+        <v>9843.600000000006</v>
+      </c>
+      <c r="D39" t="n">
+        <v>17500.079999999998</v>
+      </c>
+      <c r="E39" t="n">
+        <v>9843.600000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c s="1" r="A40" t="n">
+        <v>41539.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16728.719999999998</v>
+      </c>
+      <c r="C40" t="n">
+        <v>9225.119999999999</v>
+      </c>
+      <c r="D40" t="n">
+        <v>16728.719999999998</v>
+      </c>
+      <c r="E40" t="n">
+        <v>9225.119999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c s="1" r="A41" t="n">
+        <v>41546.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>16597.20000000001</v>
+      </c>
+      <c r="C41" t="n">
+        <v>9214.559999999998</v>
+      </c>
+      <c r="D41" t="n">
+        <v>16597.20000000001</v>
+      </c>
+      <c r="E41" t="n">
+        <v>9214.559999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c s="1" r="A42" t="n">
+        <v>41553.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>16963.92000000001</v>
+      </c>
+      <c r="C42" t="n">
+        <v>9584.159999999994</v>
+      </c>
+      <c r="D42" t="n">
+        <v>16963.92000000001</v>
+      </c>
+      <c r="E42" t="n">
+        <v>9584.159999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c s="1" r="A43" t="n">
+        <v>41560.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>15799.919999999991</v>
+      </c>
+      <c r="C43" t="n">
+        <v>9262.560000000003</v>
+      </c>
+      <c r="D43" t="n">
+        <v>15799.919999999991</v>
+      </c>
+      <c r="E43" t="n">
+        <v>9262.560000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c s="1" r="A44" t="n">
+        <v>41567.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>15060.480000000003</v>
+      </c>
+      <c r="C44" t="n">
+        <v>9060.720000000003</v>
+      </c>
+      <c r="D44" t="n">
+        <v>15060.480000000003</v>
+      </c>
+      <c r="E44" t="n">
+        <v>9060.720000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c s="1" r="A45" t="n">
+        <v>41574.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>15119.75999999999</v>
+      </c>
+      <c r="C45" t="n">
+        <v>9382.800000000001</v>
+      </c>
+      <c r="D45" t="n">
+        <v>15119.75999999999</v>
+      </c>
+      <c r="E45" t="n">
+        <v>9382.800000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c s="1" r="A46" t="n">
+        <v>41581.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>15062.640000000003</v>
+      </c>
+      <c r="C46" t="n">
+        <v>9506.639999999994</v>
+      </c>
+      <c r="D46" t="n">
+        <v>15062.640000000003</v>
+      </c>
+      <c r="E46" t="n">
+        <v>9506.639999999994</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c s="1" r="A47" t="n">
+        <v>41588.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>15123.360000000004</v>
+      </c>
+      <c r="C47" t="n">
+        <v>9651.6</v>
+      </c>
+      <c r="D47" t="n">
+        <v>15123.360000000004</v>
+      </c>
+      <c r="E47" t="n">
+        <v>9651.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c s="1" r="A48" t="n">
+        <v>41595.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>15275.280000000002</v>
+      </c>
+      <c r="C48" t="n">
+        <v>10138.080000000002</v>
+      </c>
+      <c r="D48" t="n">
+        <v>15275.280000000002</v>
+      </c>
+      <c r="E48" t="n">
+        <v>10138.080000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c s="1" r="A49" t="n">
+        <v>41602.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>15326.159999999994</v>
+      </c>
+      <c r="C49" t="n">
+        <v>9971.759999999987</v>
+      </c>
+      <c r="D49" t="n">
+        <v>15326.159999999994</v>
+      </c>
+      <c r="E49" t="n">
+        <v>9971.759999999987</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c s="1" r="A50" t="n">
+        <v>41609.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>12604.079999999996</v>
+      </c>
+      <c r="C50" t="n">
+        <v>9333.599999999997</v>
+      </c>
+      <c r="D50" t="n">
+        <v>12604.079999999996</v>
+      </c>
+      <c r="E50" t="n">
+        <v>9333.599999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c s="1" r="A51" t="n">
+        <v>41616.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>15282.240000000005</v>
+      </c>
+      <c r="C51" t="n">
+        <v>9797.040000000005</v>
+      </c>
+      <c r="D51" t="n">
+        <v>15282.240000000005</v>
+      </c>
+      <c r="E51" t="n">
+        <v>9797.040000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c s="1" r="A52" t="n">
+        <v>41623.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>15029.519999999982</v>
+      </c>
+      <c r="C52" t="n">
+        <v>9786.240000000002</v>
+      </c>
+      <c r="D52" t="n">
+        <v>15029.519999999982</v>
+      </c>
+      <c r="E52" t="n">
+        <v>9786.240000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c s="1" r="A53" t="n">
+        <v>41630.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>15185.28</v>
+      </c>
+      <c r="C53" t="n">
+        <v>9817.920000000007</v>
+      </c>
+      <c r="D53" t="n">
+        <v>15185.28</v>
+      </c>
+      <c r="E53" t="n">
+        <v>9817.920000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c s="1" r="A54" t="n">
+        <v>41637.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>12444.48</v>
+      </c>
+      <c r="C54" t="n">
+        <v>8983.440000000008</v>
+      </c>
+      <c r="D54" t="n">
+        <v>12444.48</v>
+      </c>
+      <c r="E54" t="n">
+        <v>8983.440000000008</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>